<commit_message>
switched to py 3.11
</commit_message>
<xml_diff>
--- a/models/metrics_file.xlsx
+++ b/models/metrics_file.xlsx
@@ -470,16 +470,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9595728451563692</v>
+        <v>0.9610983981693364</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9603048756969134</v>
+        <v>0.9614686212176559</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9595728451563692</v>
+        <v>0.9610983981693364</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9586412753988786</v>
+        <v>0.9602613857752854</v>
       </c>
     </row>
     <row r="3">
@@ -492,16 +492,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9799771167048055</v>
+        <v>0.9794050343249427</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9802051708731796</v>
+        <v>0.9795578020533958</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9799771167048055</v>
+        <v>0.9794050343249427</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9795352373269315</v>
+        <v>0.9790161131238534</v>
       </c>
     </row>
     <row r="4">
@@ -514,16 +514,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9992372234935164</v>
+        <v>0.9988558352402745</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9992378072138199</v>
+        <v>0.9988571491136828</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9992372234935164</v>
+        <v>0.9988558352402745</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9991972233475304</v>
+        <v>0.9987781526637115</v>
       </c>
     </row>
     <row r="5">
@@ -536,16 +536,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9513729977116705</v>
+        <v>0.9590007627765065</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9517977840797013</v>
+        <v>0.9590672423841434</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9513729977116705</v>
+        <v>0.9590007627765065</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9511717820125447</v>
+        <v>0.9589334073701533</v>
       </c>
     </row>
     <row r="6">
@@ -558,16 +558,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9824561403508771</v>
+        <v>0.982837528604119</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9825977260543096</v>
+        <v>0.9830387022797661</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9824561403508771</v>
+        <v>0.982837528604119</v>
       </c>
       <c r="F6" t="n">
-        <v>0.981488530600351</v>
+        <v>0.981974680149756</v>
       </c>
     </row>
     <row r="7">
@@ -580,16 +580,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9891304347826086</v>
+        <v>0.9893211289092296</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9891966387162929</v>
+        <v>0.9893029321775226</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9891304347826086</v>
+        <v>0.9893211289092296</v>
       </c>
       <c r="F7" t="n">
-        <v>0.988525640446135</v>
+        <v>0.9888442183535571</v>
       </c>
     </row>
     <row r="8">
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9938977879481312</v>
+        <v>0.9937070938215103</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9938851259292474</v>
+        <v>0.9936993144018478</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9938977879481312</v>
+        <v>0.9937070938215103</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9935702286878385</v>
+        <v>0.9933860189153357</v>
       </c>
     </row>
     <row r="9">
@@ -624,16 +624,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9963768115942029</v>
+        <v>0.9975209763539283</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9963901321398124</v>
+        <v>0.9974982465586499</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9963768115942029</v>
+        <v>0.9975209763539283</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9961788596186867</v>
+        <v>0.9974386488620747</v>
       </c>
     </row>
     <row r="10">
@@ -646,16 +646,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9937070938215103</v>
+        <v>0.9950419527078566</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9937479568486435</v>
+        <v>0.9950334815486824</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9937070938215103</v>
+        <v>0.9950419527078566</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9934264942494861</v>
+        <v>0.9948618772884045</v>
       </c>
     </row>
     <row r="11">
@@ -690,16 +690,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.990465293668955</v>
+        <v>0.9900839054157132</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9905224097841747</v>
+        <v>0.9901883276349078</v>
       </c>
       <c r="E12" t="n">
-        <v>0.990465293668955</v>
+        <v>0.9900839054157132</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9901070479068079</v>
+        <v>0.9897218683393449</v>
       </c>
     </row>
     <row r="13">
@@ -712,16 +712,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.9832189168573608</v>
+        <v>0.9879862700228833</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9832201590786473</v>
+        <v>0.9879331871168294</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9832189168573608</v>
+        <v>0.9879862700228833</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9827701826134044</v>
+        <v>0.987792648483144</v>
       </c>
     </row>
     <row r="14">
@@ -734,16 +734,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.9853165522501907</v>
+        <v>0.9858886346300534</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9854185021883204</v>
+        <v>0.985890248708102</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9853165522501907</v>
+        <v>0.9858886346300534</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9847566585257136</v>
+        <v>0.9854588633226952</v>
       </c>
     </row>
     <row r="15">
@@ -756,16 +756,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.9969488939740656</v>
+        <v>0.9973302822273074</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9969232772979159</v>
+        <v>0.9973375158345879</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9969488939740656</v>
+        <v>0.9973302822273074</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9968282190819312</v>
+        <v>0.997220854841857</v>
       </c>
     </row>
     <row r="16">
@@ -778,16 +778,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.9946605644546148</v>
+        <v>0.9958047292143402</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9946896113159459</v>
+        <v>0.9957829141587861</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9946605644546148</v>
+        <v>0.9958047292143402</v>
       </c>
       <c r="F16" t="n">
-        <v>0.994331124815392</v>
+        <v>0.9956215277043468</v>
       </c>
     </row>
     <row r="17">
@@ -800,16 +800,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.9971395881006865</v>
+        <v>0.9969488939740656</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9971478297792286</v>
+        <v>0.9969582928374492</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9971395881006865</v>
+        <v>0.9969488939740656</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9969059032594787</v>
+        <v>0.996740826209381</v>
       </c>
     </row>
     <row r="18">
@@ -822,16 +822,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.9912280701754386</v>
+        <v>0.9956140350877193</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9913070347100629</v>
+        <v>0.9956338265715299</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9912280701754386</v>
+        <v>0.9956140350877193</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9906053706736443</v>
+        <v>0.9954598818556766</v>
       </c>
     </row>
     <row r="19">
@@ -844,16 +844,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.9910373760488177</v>
+        <v>0.9918001525553013</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9910676521305324</v>
+        <v>0.9918703343706122</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9910373760488177</v>
+        <v>0.9918001525553013</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9905594524006556</v>
+        <v>0.9914527698556737</v>
       </c>
     </row>
     <row r="20">
@@ -866,16 +866,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.971205186880244</v>
+        <v>0.9729214340198322</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9719134071599742</v>
+        <v>0.9737448079746895</v>
       </c>
       <c r="E20" t="n">
-        <v>0.971205186880244</v>
+        <v>0.9729214340198322</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9696769021362707</v>
+        <v>0.9716400846631509</v>
       </c>
     </row>
     <row r="21">
@@ -888,16 +888,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.9881769641495042</v>
+        <v>0.9864607170099161</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9882719908148445</v>
+        <v>0.9865962758749373</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9881769641495042</v>
+        <v>0.9864607170099161</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9875904614636357</v>
+        <v>0.985730747981579</v>
       </c>
     </row>
     <row r="22">
@@ -910,16 +910,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.9898932112890922</v>
+        <v>0.988558352402746</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9898891438520425</v>
+        <v>0.9886318138113294</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9898932112890922</v>
+        <v>0.988558352402746</v>
       </c>
       <c r="F22" t="n">
-        <v>0.98934063345762</v>
+        <v>0.9878605666067279</v>
       </c>
     </row>
     <row r="23">
@@ -932,16 +932,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.9921815408085431</v>
+        <v>0.9900839054157132</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9921418500675491</v>
+        <v>0.9900893476441833</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9921815408085431</v>
+        <v>0.9900839054157132</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9919095677280201</v>
+        <v>0.9896077043630818</v>
       </c>
     </row>
     <row r="24">
@@ -954,16 +954,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.9959954233409611</v>
+        <v>0.9973302822273074</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9960117495125472</v>
+        <v>0.9973375298613616</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9959954233409611</v>
+        <v>0.9973302822273074</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9957963825207328</v>
+        <v>0.9972326922134557</v>
       </c>
     </row>
     <row r="25">
@@ -976,16 +976,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.9994279176201373</v>
+        <v>0.9986651411136537</v>
       </c>
       <c r="D25" t="n">
-        <v>0.999428246340141</v>
+        <v>0.9986669345900845</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9994279176201373</v>
+        <v>0.9986651411136537</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9994104870978412</v>
+        <v>0.9986032963694753</v>
       </c>
     </row>
     <row r="26">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.9982837528604119</v>
+        <v>0.9984744469870328</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9982867221461206</v>
+        <v>0.9984767939916682</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9982837528604119</v>
+        <v>0.9984744469870328</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9982014516081099</v>
+        <v>0.9984114694810127</v>
       </c>
     </row>
     <row r="27">
@@ -1020,16 +1020,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.9992372234935164</v>
+        <v>0.9988558352402745</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9992378072138199</v>
+        <v>0.9988571491136828</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9992372234935164</v>
+        <v>0.9988558352402745</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9991972233475304</v>
+        <v>0.9987781526637115</v>
       </c>
     </row>
     <row r="28">
@@ -1042,16 +1042,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.9988558352402745</v>
+        <v>0.9979023646071701</v>
       </c>
       <c r="D28" t="n">
-        <v>0.998857156955438</v>
+        <v>0.9979068070386914</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9988558352402745</v>
+        <v>0.9979023646071701</v>
       </c>
       <c r="F28" t="n">
-        <v>0.9988237838385262</v>
+        <v>0.9977995395035014</v>
       </c>
     </row>
     <row r="29">
@@ -1064,16 +1064,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.9910373760488177</v>
+        <v>0.9900839054157132</v>
       </c>
       <c r="D29" t="n">
-        <v>0.9911204123834729</v>
+        <v>0.9901272713322234</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9910373760488177</v>
+        <v>0.9900839054157132</v>
       </c>
       <c r="F29" t="n">
-        <v>0.9905167878803487</v>
+        <v>0.9895068038989967</v>
       </c>
     </row>
     <row r="30">
@@ -1086,16 +1086,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.9744469870327994</v>
+        <v>0.9731121281464531</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9744708127006981</v>
+        <v>0.9733276997163469</v>
       </c>
       <c r="E30" t="n">
-        <v>0.9744469870327994</v>
+        <v>0.9731121281464531</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9742492053813423</v>
+        <v>0.9728516613925116</v>
       </c>
     </row>
     <row r="31">
@@ -1108,16 +1108,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.9898932112890922</v>
+        <v>0.9887490465293669</v>
       </c>
       <c r="D31" t="n">
-        <v>0.9899390364995758</v>
+        <v>0.9887600503347537</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9898932112890922</v>
+        <v>0.9887490465293669</v>
       </c>
       <c r="F31" t="n">
-        <v>0.98959753153796</v>
+        <v>0.9884351757961887</v>
       </c>
     </row>
     <row r="32">
@@ -1130,16 +1130,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.9832189168573608</v>
+        <v>0.9874141876430206</v>
       </c>
       <c r="D32" t="n">
-        <v>0.9830433084551015</v>
+        <v>0.987258216629961</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9832189168573608</v>
+        <v>0.9874141876430206</v>
       </c>
       <c r="F32" t="n">
-        <v>0.9826517390711269</v>
+        <v>0.9871746138310818</v>
       </c>
     </row>
     <row r="33">
@@ -1152,16 +1152,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.9982837528604119</v>
+        <v>0.9986651411136537</v>
       </c>
       <c r="D33" t="n">
-        <v>0.9982867278650838</v>
+        <v>0.9986669390763637</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9982837528604119</v>
+        <v>0.9986651411136537</v>
       </c>
       <c r="F33" t="n">
-        <v>0.9982161511317338</v>
+        <v>0.998619333421091</v>
       </c>
     </row>
     <row r="34">
@@ -1174,16 +1174,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.9940884820747521</v>
+        <v>0.9935163996948894</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9940771927683076</v>
+        <v>0.9934801213779205</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9940884820747521</v>
+        <v>0.9935163996948894</v>
       </c>
       <c r="F34" t="n">
-        <v>0.9940271802031352</v>
+        <v>0.9934881668919573</v>
       </c>
     </row>
     <row r="35">
@@ -1199,13 +1199,13 @@
         <v>0.9963768115942029</v>
       </c>
       <c r="D35" t="n">
-        <v>0.996390165731877</v>
+        <v>0.9963536549221774</v>
       </c>
       <c r="E35" t="n">
         <v>0.9963768115942029</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9962054340089406</v>
+        <v>0.9962295767840115</v>
       </c>
     </row>
     <row r="36">
@@ -1218,16 +1218,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.9877955758962624</v>
+        <v>0.9887490465293669</v>
       </c>
       <c r="D36" t="n">
-        <v>0.987885407786303</v>
+        <v>0.9888246208345635</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9877955758962624</v>
+        <v>0.9887490465293669</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9870283689790077</v>
+        <v>0.9881307176983142</v>
       </c>
     </row>
     <row r="37">
@@ -1240,16 +1240,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.9729214340198322</v>
+        <v>0.9731121281464531</v>
       </c>
       <c r="D37" t="n">
-        <v>0.9734874411407183</v>
+        <v>0.9733036207132412</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9729214340198322</v>
+        <v>0.9731121281464531</v>
       </c>
       <c r="F37" t="n">
-        <v>0.9722181116157896</v>
+        <v>0.9725707615990664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>